<commit_message>
added EnrollCourseTest,Cart_page,EnrollPage,added few methods in HomePage
</commit_message>
<xml_diff>
--- a/testdata/Data.xlsx
+++ b/testdata/Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/swati/Desktop/BreakOutSessionDec2024/AugFramework/testdata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4a21da591722a5a3/Desktop/ECLIPSE/SeleniumTraining_Jul/AugFramework/testdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D8D4871-7BC0-2441-AA4F-9EB21D7C20B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="13" documentId="13_ncr:1_{7D8D4871-7BC0-2441-AA4F-9EB21D7C20B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5D3ECAA7-E6E3-49B1-9CDC-6D6C25D01F92}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="new_users" sheetId="5" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
   <si>
     <t>Username</t>
   </si>
@@ -80,6 +80,21 @@
   </si>
   <si>
     <t>ora20@gmail.com</t>
+  </si>
+  <si>
+    <t>Course</t>
+  </si>
+  <si>
+    <t>Hyderabad</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>Selenium</t>
   </si>
 </sst>
 </file>
@@ -148,7 +163,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -156,6 +171,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -354,11 +370,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2BB1766-F063-F049-BAE8-AE90D139D96C}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+    <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.33203125" customWidth="1"/>
     <col min="2" max="2" width="22.6640625" customWidth="1"/>
@@ -366,7 +382,7 @@
     <col min="4" max="4" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
@@ -389,7 +405,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -427,12 +443,12 @@
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.5" customWidth="1"/>
+    <col min="1" max="1" width="26.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -440,7 +456,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -464,11 +480,53 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2">
+        <v>1234567891</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -479,30 +537,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
-  <sheetData/>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter>
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
added AddCourseTest,coursepage,selectValueFromList,CheckValueIsPresentInList,findElements methods in utility
</commit_message>
<xml_diff>
--- a/testdata/Data.xlsx
+++ b/testdata/Data.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4a21da591722a5a3/Desktop/ECLIPSE/SeleniumTraining_Jul/AugFramework/testdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="13_ncr:1_{7D8D4871-7BC0-2441-AA4F-9EB21D7C20B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5D3ECAA7-E6E3-49B1-9CDC-6D6C25D01F92}"/>
+  <xr:revisionPtr revIDLastSave="20" documentId="13_ncr:1_{7D8D4871-7BC0-2441-AA4F-9EB21D7C20B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{96C27AEB-B9FE-4D0E-A5E4-A0670FF48D1F}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="252" yWindow="24" windowWidth="22788" windowHeight="12216" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="new_users" sheetId="5" r:id="rId1"/>
     <sheet name="login_details" sheetId="1" r:id="rId2"/>
     <sheet name="courses_details" sheetId="2" r:id="rId3"/>
-    <sheet name="category_details" sheetId="3" r:id="rId4"/>
-    <sheet name="product_details" sheetId="4" r:id="rId5"/>
+    <sheet name="addCourse_details" sheetId="6" r:id="rId4"/>
+    <sheet name="category_details" sheetId="3" r:id="rId5"/>
+    <sheet name="product_details" sheetId="4" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="34">
   <si>
     <t>Username</t>
   </si>
@@ -95,13 +96,49 @@
   </si>
   <si>
     <t>Selenium</t>
+  </si>
+  <si>
+    <t>File</t>
+  </si>
+  <si>
+    <t>C:\\Users\\PRADE\\OneDrive\\Desktop\\uploadFile.jpg</t>
+  </si>
+  <si>
+    <t>CourseName</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Instructor</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Rithika</t>
+  </si>
+  <si>
+    <t>Start_dt</t>
+  </si>
+  <si>
+    <t>End_dt</t>
+  </si>
+  <si>
+    <t>ETL</t>
+  </si>
+  <si>
+    <t>CategoryName</t>
+  </si>
+  <si>
+    <t>InformaticaDB</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -128,6 +165,12 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF2A00FF"/>
+      <name val="Courier New"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="4">
@@ -163,7 +206,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -172,6 +215,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -482,7 +526,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -521,6 +565,78 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75AC087D-02D6-47C5-B3B7-1A69804AC6EC}">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="70.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2">
+        <v>10000</v>
+      </c>
+      <c r="F2">
+        <v>20</v>
+      </c>
+      <c r="G2">
+        <v>5</v>
+      </c>
+      <c r="H2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -537,7 +653,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>

<commit_message>
added all xml files in pom
</commit_message>
<xml_diff>
--- a/testdata/Data.xlsx
+++ b/testdata/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4a21da591722a5a3/Desktop/ECLIPSE/SeleniumTraining_Jul/AugFramework/testdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="30" documentId="13_ncr:1_{7D8D4871-7BC0-2441-AA4F-9EB21D7C20B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{98DD4E2A-5B88-4B66-B589-5827B1643AE1}"/>
+  <xr:revisionPtr revIDLastSave="32" documentId="13_ncr:1_{7D8D4871-7BC0-2441-AA4F-9EB21D7C20B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F08F7E01-6635-4CED-9D88-F997EDA28FCB}"/>
   <bookViews>
     <workbookView xWindow="252" yWindow="24" windowWidth="22788" windowHeight="12216" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -137,10 +137,10 @@
     <t>Informatica</t>
   </si>
   <si>
-    <t>ManualTesting</t>
-  </si>
-  <si>
     <t>Susmitha</t>
+  </si>
+  <si>
+    <t>Teamcity</t>
   </si>
 </sst>
 </file>
@@ -431,7 +431,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -467,7 +467,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>14</v>
@@ -476,7 +476,7 @@
         <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E2" t="s">
         <v>11</v>
@@ -585,7 +585,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -644,7 +644,7 @@
         <v>5</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modified utility and to run on grid
</commit_message>
<xml_diff>
--- a/testdata/Data.xlsx
+++ b/testdata/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4a21da591722a5a3/Desktop/ECLIPSE/SeleniumTraining_Jul/AugFramework/testdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="32" documentId="13_ncr:1_{7D8D4871-7BC0-2441-AA4F-9EB21D7C20B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F08F7E01-6635-4CED-9D88-F997EDA28FCB}"/>
+  <xr:revisionPtr revIDLastSave="33" documentId="13_ncr:1_{7D8D4871-7BC0-2441-AA4F-9EB21D7C20B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3AF7674E-0D63-44D5-BCCC-003273BDCFD7}"/>
   <bookViews>
     <workbookView xWindow="252" yWindow="24" windowWidth="22788" windowHeight="12216" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="38">
   <si>
     <t>Username</t>
   </si>
@@ -141,6 +141,9 @@
   </si>
   <si>
     <t>Teamcity</t>
+  </si>
+  <si>
+    <t>Java</t>
   </si>
 </sst>
 </file>
@@ -585,7 +588,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -644,7 +647,7 @@
         <v>5</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>